<commit_message>
Market Cap in EUR
</commit_message>
<xml_diff>
--- a/EFI/CODE/input/anagrafiche/strategie.xlsx
+++ b/EFI/CODE/input/anagrafiche/strategie.xlsx
@@ -515,6 +515,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0066"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2703,10 +2708,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0066"/>
+  </sheetPr>
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>